<commit_message>
Fill in most of the text
</commit_message>
<xml_diff>
--- a/indicators/NO_BFLY_001/metadata.xlsx
+++ b/indicators/NO_BFLY_001/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anders.kolstad\Github\ecRxiv_butterflies\indicators\NO_BFLY_001\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB3B913-0341-4D58-BF3A-A47C7D867563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406C50C8-C979-4AA4-9C18-23EEAD5266EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="38700" windowHeight="15435" xr2:uid="{5774BAF6-AFFD-43CB-8AE5-DFBA2C21B702}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="208">
   <si>
     <t>indicatorID</t>
   </si>
@@ -687,9 +687,6 @@
     <t>NO_BFLY_001</t>
   </si>
   <si>
-    <t>Butterflies</t>
-  </si>
-  <si>
     <t>000.002</t>
   </si>
   <si>
@@ -700,13 +697,22 @@
   </si>
   <si>
     <t>https://github.com/NINAnor/ecRxiv/tree/main/indicators/NO_BFLY_001</t>
+  </si>
+  <si>
+    <t>Butterflies in semi-natural grasslands</t>
+  </si>
+  <si>
+    <t>Reference levels</t>
+  </si>
+  <si>
+    <t>X0 and X100 defined through reference communitis made through expect elicitation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -751,6 +757,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -821,7 +833,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -832,6 +844,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1150,10 +1163,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A78FF33B-C37D-487F-A5F6-37AB2202A4CF}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,12 +1203,12 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>201</v>
+      <c r="B3" s="8" t="s">
+        <v>205</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>11</v>
@@ -1320,7 +1333,7 @@
         <v>169</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>181</v>
@@ -1334,7 +1347,7 @@
         <v>170</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>171</v>
@@ -1346,7 +1359,7 @@
         <v>188</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>185</v>
@@ -1360,7 +1373,7 @@
         <v>186</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>190</v>
@@ -1393,6 +1406,14 @@
       </c>
       <c r="D18" s="2" t="s">
         <v>198</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>